<commit_message>
Fixed some inconsistencies between the scrum board and the burndown chart
</commit_message>
<xml_diff>
--- a/SE202526/Management/Sprint3/burndown/Sprint3_Burndown.xlsx
+++ b/SE202526/Management/Sprint3/burndown/Sprint3_Burndown.xlsx
@@ -1197,8 +1197,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1308745242"/>
-        <c:axId val="1512866272"/>
+        <c:axId val="1899502934"/>
+        <c:axId val="1757060210"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1266,11 +1266,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1308745242"/>
-        <c:axId val="1512866272"/>
+        <c:axId val="1899502934"/>
+        <c:axId val="1757060210"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1308745242"/>
+        <c:axId val="1899502934"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,10 +1322,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1512866272"/>
+        <c:crossAx val="1757060210"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1512866272"/>
+        <c:axId val="1757060210"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15.0"/>
@@ -1390,7 +1390,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1308745242"/>
+        <c:crossAx val="1899502934"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1478,8 +1478,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1570117734"/>
-        <c:axId val="1525592912"/>
+        <c:axId val="1150066893"/>
+        <c:axId val="18985250"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1547,11 +1547,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1570117734"/>
-        <c:axId val="1525592912"/>
+        <c:axId val="1150066893"/>
+        <c:axId val="18985250"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1570117734"/>
+        <c:axId val="1150066893"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1603,10 +1603,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1525592912"/>
+        <c:crossAx val="18985250"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1525592912"/>
+        <c:axId val="18985250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15.0"/>
@@ -1671,7 +1671,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1570117734"/>
+        <c:crossAx val="1150066893"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1759,8 +1759,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="678014364"/>
-        <c:axId val="1030274343"/>
+        <c:axId val="1212323382"/>
+        <c:axId val="897260462"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -1828,11 +1828,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="678014364"/>
-        <c:axId val="1030274343"/>
+        <c:axId val="1212323382"/>
+        <c:axId val="897260462"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="678014364"/>
+        <c:axId val="1212323382"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1884,10 +1884,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1030274343"/>
+        <c:crossAx val="897260462"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1030274343"/>
+        <c:axId val="897260462"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16.0"/>
@@ -1952,7 +1952,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="678014364"/>
+        <c:crossAx val="1212323382"/>
         <c:majorUnit val="4.0"/>
         <c:minorUnit val="1.3333333333333333"/>
       </c:valAx>
@@ -5394,15 +5394,15 @@
         <v>0.1</v>
       </c>
       <c r="K8" s="60">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="L8" s="70" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N8" s="70">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="O8" s="71" t="s">
         <v>41</v>
@@ -5565,10 +5565,10 @@
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="60">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="G13" s="60">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H13" s="60"/>
       <c r="I13" s="32"/>
@@ -5576,11 +5576,11 @@
       <c r="K13" s="31"/>
       <c r="L13" s="70" t="str">
         <f t="shared" si="1"/>
-        <v>DONE</v>
+        <v>NOT ENOUGH WORK YET</v>
       </c>
       <c r="N13" s="70">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O13" s="71" t="s">
         <v>49</v>
@@ -6447,11 +6447,11 @@
       </c>
       <c r="F38" s="39">
         <f t="shared" si="3"/>
-        <v>1.35</v>
+        <v>1.3</v>
       </c>
       <c r="G38" s="39">
         <f t="shared" si="3"/>
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="H38" s="39">
         <f t="shared" si="3"/>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="K38" s="39">
         <f t="shared" si="3"/>
-        <v>2.4</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
@@ -6485,27 +6485,27 @@
       </c>
       <c r="F39" s="47">
         <f t="shared" si="4"/>
-        <v>13.65</v>
+        <v>13.7</v>
       </c>
       <c r="G39" s="47">
         <f t="shared" si="4"/>
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="H39" s="47">
         <f t="shared" si="4"/>
-        <v>12.6</v>
+        <v>12.7</v>
       </c>
       <c r="I39" s="48">
         <f t="shared" si="4"/>
-        <v>11.55</v>
+        <v>11.65</v>
       </c>
       <c r="J39" s="49">
         <f t="shared" si="4"/>
-        <v>8.75</v>
+        <v>8.85</v>
       </c>
       <c r="K39" s="49">
         <f t="shared" si="4"/>
-        <v>6.35</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">

</xml_diff>